<commit_message>
MAIN Project skeleton initiated
</commit_message>
<xml_diff>
--- a/schema_doc.xlsx
+++ b/schema_doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Order</t>
   </si>
@@ -81,9 +81,6 @@
     <t>ArticalName</t>
   </si>
   <si>
-    <t>Articale</t>
-  </si>
-  <si>
     <t>OrderDate</t>
   </si>
   <si>
@@ -126,21 +123,12 @@
     <t>Functional Scope description</t>
   </si>
   <si>
-    <t>customerId</t>
-  </si>
-  <si>
-    <t>serviceId</t>
-  </si>
-  <si>
     <t>articleId</t>
   </si>
   <si>
     <t>orderId</t>
   </si>
   <si>
-    <t>article_list</t>
-  </si>
-  <si>
     <t>Spring 1</t>
   </si>
   <si>
@@ -153,37 +141,112 @@
     <t>middleName</t>
   </si>
   <si>
-    <t>Avinash</t>
-  </si>
-  <si>
-    <t>Ramesh</t>
-  </si>
-  <si>
     <t>khadsan</t>
   </si>
   <si>
     <t>avish</t>
   </si>
   <si>
-    <t>###kjkjkj</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>Aniket</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>dddd</t>
+    <t>service_Id</t>
+  </si>
+  <si>
+    <t>order_article</t>
+  </si>
+  <si>
+    <t>avinash</t>
+  </si>
+  <si>
+    <t>ramesh</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>ROL01</t>
+  </si>
+  <si>
+    <t>ROL02</t>
+  </si>
+  <si>
+    <t>Viewer</t>
+  </si>
+  <si>
+    <t>User_Role</t>
+  </si>
+  <si>
+    <t>Swaraj</t>
+  </si>
+  <si>
+    <t>dssdd</t>
+  </si>
+  <si>
+    <t>jkhgjkhjk</t>
+  </si>
+  <si>
+    <t>jkhjkhkj</t>
+  </si>
+  <si>
+    <t>jhj</t>
+  </si>
+  <si>
+    <t>ROL03</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>datw</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>ArticleId</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>M:M</t>
+  </si>
+  <si>
+    <t>M:1</t>
+  </si>
+  <si>
+    <t>Spring First Schema design</t>
+  </si>
+  <si>
+    <t>BaseEntiry</t>
+  </si>
+  <si>
+    <t>createdBy</t>
+  </si>
+  <si>
+    <t>modifiedBy</t>
+  </si>
+  <si>
+    <t>createdDate</t>
+  </si>
+  <si>
+    <t>modifiedDate</t>
+  </si>
+  <si>
+    <t>swaraj</t>
   </si>
 </sst>
 </file>
@@ -221,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,8 +297,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -267,11 +360,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -284,22 +386,47 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -322,13 +449,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -369,15 +496,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -385,9 +512,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2562225" y="857250"/>
-          <a:ext cx="3076575" cy="12700"/>
+        <a:xfrm flipV="1">
+          <a:off x="2676525" y="1631950"/>
+          <a:ext cx="3613785" cy="6350"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -420,13 +547,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -441,7 +568,7 @@
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 39399"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -468,16 +595,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1219201</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>600080</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152403</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -486,12 +613,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="6315076" y="1457325"/>
-          <a:ext cx="1743075" cy="542925"/>
+          <a:off x="5310189" y="1271587"/>
+          <a:ext cx="3105153" cy="2276479"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -273"/>
+            <a:gd name="adj1" fmla="val 81595"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -520,13 +647,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -568,13 +695,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -596,6 +723,337 @@
           <a:headEnd type="arrow"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Curved Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2647950" y="276225"/>
+          <a:ext cx="1885950" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Curved Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3328988" y="557213"/>
+          <a:ext cx="1390650" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 7534"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Curved Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6172200" y="304800"/>
+          <a:ext cx="1914525" cy="1123950"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Curved Connector 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6210300" y="247650"/>
+          <a:ext cx="3924300" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 72330"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2981325" y="2581275"/>
+          <a:ext cx="361951" cy="9526"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2981325" y="323850"/>
+          <a:ext cx="28575" cy="2257425"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3000375" y="295275"/>
+          <a:ext cx="1504950" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -904,407 +1362,676 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P24"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+    </row>
+    <row r="2" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="16"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="16"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="I4" s="12" t="s">
+      <c r="D8" s="27"/>
+      <c r="I8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="L4" s="11" t="s">
+      <c r="J8" s="28"/>
+      <c r="L8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="11"/>
-      <c r="O4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="11"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="M8" s="28"/>
+      <c r="O8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="28"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="J9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="M9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="P9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="15"/>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="I6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="15"/>
+      <c r="R10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F11" s="1" t="s">
+      <c r="G14" s="28"/>
+      <c r="L14" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="22"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N14" s="1">
-        <v>2</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1</v>
-      </c>
-      <c r="P14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F15" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="1">
-        <v>3</v>
-      </c>
-      <c r="O15" s="1">
-        <v>1</v>
-      </c>
-      <c r="P15" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E18" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="J28" t="s">
+        <v>5</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F20" s="4" t="s">
+      <c r="H29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J31" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M31" s="1">
+        <v>2</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M20" s="13"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I21" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="L21" s="1">
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J32" s="9">
         <v>1</v>
       </c>
-      <c r="M21" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I22" s="1">
+      <c r="K32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L32">
         <v>1</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" s="1">
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D33" s="9">
         <v>1</v>
       </c>
-      <c r="M22" s="1">
+      <c r="E33" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
+      <c r="G33" s="9">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="1">
-        <v>2</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L23">
-        <v>2</v>
-      </c>
-      <c r="M23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+      <c r="J33" s="9">
+        <v>1</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L33" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D34" s="12">
+        <v>2</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="12">
+        <v>2</v>
+      </c>
+      <c r="G34" s="12">
+        <v>1</v>
+      </c>
+      <c r="J34" s="11">
+        <v>2</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J35" s="11">
+        <v>2</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="N12:P12"/>
+  <mergeCells count="16">
+    <mergeCell ref="E1:P1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A27:R27"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="O8:P8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1327,10 +2054,10 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="C3" s="9"/>
     </row>
@@ -1339,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1347,7 +2074,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1355,7 +2082,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RLB-main country flow initated
</commit_message>
<xml_diff>
--- a/schema_doc.xlsx
+++ b/schema_doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>Order</t>
   </si>
@@ -247,6 +247,24 @@
   </si>
   <si>
     <t>swaraj</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>China</t>
   </si>
 </sst>
 </file>
@@ -405,6 +423,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,15 +442,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1362,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,29 +1399,29 @@
       <c r="B1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="27"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
@@ -1504,22 +1522,22 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="I8" s="28" t="s">
+      <c r="D8" s="24"/>
+      <c r="I8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="L8" s="28" t="s">
+      <c r="J8" s="29"/>
+      <c r="L8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="28"/>
-      <c r="O8" s="28" t="s">
+      <c r="M8" s="29"/>
+      <c r="O8" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="28"/>
+      <c r="P8" s="29"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1561,10 +1579,10 @@
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="29"/>
       <c r="I10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1650,26 +1668,32 @@
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="29"/>
       <c r="L14" s="21" t="s">
         <v>68</v>
       </c>
       <c r="M14" s="22"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="28"/>
+      <c r="J15" s="29"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
@@ -1685,9 +1709,9 @@
       <c r="J16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
@@ -1743,8 +1767,8 @@
       <c r="G20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
@@ -1781,8 +1805,8 @@
       <c r="G24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F25" s="4" t="s">
@@ -1791,8 +1815,8 @@
       <c r="G25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
@@ -1805,44 +1829,44 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
       <c r="J28" t="s">
         <v>5</v>
       </c>
-      <c r="M28" s="23" t="s">
+      <c r="M28" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="N28" s="23"/>
+      <c r="N28" s="25"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
@@ -1946,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D33" s="9">
         <v>1</v>
       </c>
@@ -1972,7 +1996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D34" s="12">
         <v>2</v>
       </c>
@@ -1995,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J35" s="11">
         <v>2</v>
       </c>
@@ -2006,13 +2030,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
     </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
RLB-main  Address schema added
</commit_message>
<xml_diff>
--- a/schema_doc.xlsx
+++ b/schema_doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
   <si>
     <t>Order</t>
   </si>
@@ -246,9 +246,6 @@
     <t>modifiedDate</t>
   </si>
   <si>
-    <t>swaraj</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -265,6 +262,21 @@
   </si>
   <si>
     <t>China</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Tehsil</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -391,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,6 +459,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,13 +480,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -513,13 +528,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -563,13 +578,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -613,13 +628,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1219201</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>600080</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>152403</xdr:rowOff>
@@ -663,13 +678,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -711,13 +726,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
@@ -761,13 +776,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -809,13 +824,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
@@ -859,13 +874,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -907,13 +922,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -957,13 +972,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>66676</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
@@ -1004,13 +1019,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -1048,13 +1063,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -1088,6 +1103,606 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Curved Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1228725" y="676275"/>
+          <a:ext cx="590550" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Curved Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1228725" y="1066800"/>
+          <a:ext cx="561975" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Curved Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="1009650" y="1428751"/>
+          <a:ext cx="981075" cy="619125"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98544"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Curved Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="747713" y="1909763"/>
+          <a:ext cx="1533525" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Curved Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="623887" y="2319338"/>
+          <a:ext cx="2019300" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133791</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Freeform 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057525" y="885825"/>
+          <a:ext cx="628650" cy="1914966"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 628650"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1914966"/>
+            <a:gd name="connsiteX1" fmla="*/ 171450 w 628650"/>
+            <a:gd name="connsiteY1" fmla="*/ 190500 h 1914966"/>
+            <a:gd name="connsiteX2" fmla="*/ 200025 w 628650"/>
+            <a:gd name="connsiteY2" fmla="*/ 247650 h 1914966"/>
+            <a:gd name="connsiteX3" fmla="*/ 190500 w 628650"/>
+            <a:gd name="connsiteY3" fmla="*/ 628650 h 1914966"/>
+            <a:gd name="connsiteX4" fmla="*/ 180975 w 628650"/>
+            <a:gd name="connsiteY4" fmla="*/ 742950 h 1914966"/>
+            <a:gd name="connsiteX5" fmla="*/ 152400 w 628650"/>
+            <a:gd name="connsiteY5" fmla="*/ 838200 h 1914966"/>
+            <a:gd name="connsiteX6" fmla="*/ 142875 w 628650"/>
+            <a:gd name="connsiteY6" fmla="*/ 1247775 h 1914966"/>
+            <a:gd name="connsiteX7" fmla="*/ 133350 w 628650"/>
+            <a:gd name="connsiteY7" fmla="*/ 1276350 h 1914966"/>
+            <a:gd name="connsiteX8" fmla="*/ 114300 w 628650"/>
+            <a:gd name="connsiteY8" fmla="*/ 1400175 h 1914966"/>
+            <a:gd name="connsiteX9" fmla="*/ 133350 w 628650"/>
+            <a:gd name="connsiteY9" fmla="*/ 1495425 h 1914966"/>
+            <a:gd name="connsiteX10" fmla="*/ 152400 w 628650"/>
+            <a:gd name="connsiteY10" fmla="*/ 1571625 h 1914966"/>
+            <a:gd name="connsiteX11" fmla="*/ 171450 w 628650"/>
+            <a:gd name="connsiteY11" fmla="*/ 1600200 h 1914966"/>
+            <a:gd name="connsiteX12" fmla="*/ 180975 w 628650"/>
+            <a:gd name="connsiteY12" fmla="*/ 1628775 h 1914966"/>
+            <a:gd name="connsiteX13" fmla="*/ 295275 w 628650"/>
+            <a:gd name="connsiteY13" fmla="*/ 1724025 h 1914966"/>
+            <a:gd name="connsiteX14" fmla="*/ 352425 w 628650"/>
+            <a:gd name="connsiteY14" fmla="*/ 1781175 h 1914966"/>
+            <a:gd name="connsiteX15" fmla="*/ 390525 w 628650"/>
+            <a:gd name="connsiteY15" fmla="*/ 1838325 h 1914966"/>
+            <a:gd name="connsiteX16" fmla="*/ 419100 w 628650"/>
+            <a:gd name="connsiteY16" fmla="*/ 1857375 h 1914966"/>
+            <a:gd name="connsiteX17" fmla="*/ 447675 w 628650"/>
+            <a:gd name="connsiteY17" fmla="*/ 1885950 h 1914966"/>
+            <a:gd name="connsiteX18" fmla="*/ 476250 w 628650"/>
+            <a:gd name="connsiteY18" fmla="*/ 1895475 h 1914966"/>
+            <a:gd name="connsiteX19" fmla="*/ 504825 w 628650"/>
+            <a:gd name="connsiteY19" fmla="*/ 1914525 h 1914966"/>
+            <a:gd name="connsiteX20" fmla="*/ 619125 w 628650"/>
+            <a:gd name="connsiteY20" fmla="*/ 1905000 h 1914966"/>
+            <a:gd name="connsiteX21" fmla="*/ 628650 w 628650"/>
+            <a:gd name="connsiteY21" fmla="*/ 1905000 h 1914966"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="628650" h="1914966">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="149539" y="149539"/>
+                <a:pt x="98481" y="81046"/>
+                <a:pt x="171450" y="190500"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="196069" y="227429"/>
+                <a:pt x="186880" y="208215"/>
+                <a:pt x="200025" y="247650"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="196850" y="374650"/>
+                <a:pt x="195383" y="501704"/>
+                <a:pt x="190500" y="628650"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="189031" y="666854"/>
+                <a:pt x="186938" y="705186"/>
+                <a:pt x="180975" y="742950"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="177704" y="763668"/>
+                <a:pt x="161182" y="811853"/>
+                <a:pt x="152400" y="838200"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="149225" y="974725"/>
+                <a:pt x="148807" y="1111342"/>
+                <a:pt x="142875" y="1247775"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="142439" y="1257806"/>
+                <a:pt x="134877" y="1266427"/>
+                <a:pt x="133350" y="1276350"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="112302" y="1413163"/>
+                <a:pt x="137227" y="1331395"/>
+                <a:pt x="114300" y="1400175"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="132965" y="1512163"/>
+                <a:pt x="114405" y="1410171"/>
+                <a:pt x="133350" y="1495425"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="137697" y="1514988"/>
+                <a:pt x="142188" y="1551200"/>
+                <a:pt x="152400" y="1571625"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="157520" y="1581864"/>
+                <a:pt x="166330" y="1589961"/>
+                <a:pt x="171450" y="1600200"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="175940" y="1609180"/>
+                <a:pt x="174811" y="1620850"/>
+                <a:pt x="180975" y="1628775"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="220465" y="1679548"/>
+                <a:pt x="244475" y="1690158"/>
+                <a:pt x="295275" y="1724025"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="317691" y="1738969"/>
+                <a:pt x="333375" y="1762125"/>
+                <a:pt x="352425" y="1781175"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="368614" y="1797364"/>
+                <a:pt x="371475" y="1825625"/>
+                <a:pt x="390525" y="1838325"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="400050" y="1844675"/>
+                <a:pt x="410306" y="1850046"/>
+                <a:pt x="419100" y="1857375"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="429448" y="1865999"/>
+                <a:pt x="436467" y="1878478"/>
+                <a:pt x="447675" y="1885950"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="456029" y="1891519"/>
+                <a:pt x="466725" y="1892300"/>
+                <a:pt x="476250" y="1895475"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="485775" y="1901825"/>
+                <a:pt x="493403" y="1913764"/>
+                <a:pt x="504825" y="1914525"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="542972" y="1917068"/>
+                <a:pt x="581006" y="1907932"/>
+                <a:pt x="619125" y="1905000"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="622291" y="1904756"/>
+                <a:pt x="625475" y="1905000"/>
+                <a:pt x="628650" y="1905000"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Freeform 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="895350"/>
+          <a:ext cx="9525" cy="76200"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 9525"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 76200"/>
+            <a:gd name="connsiteX1" fmla="*/ 9525 w 9525"/>
+            <a:gd name="connsiteY1" fmla="*/ 76200 h 76200"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="9525" h="76200">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="9525" y="76200"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1380,28 +1995,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="B1" s="23" t="s">
         <v>39</v>
       </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -1413,429 +2031,551 @@
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
       <c r="P1" s="23"/>
-    </row>
-    <row r="2" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="24"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+    </row>
+    <row r="2" spans="1:22" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="16"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="K2" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="24"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="16"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19" t="s">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="D3" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="L3" s="19" t="s">
+        <v>2</v>
+      </c>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>2</v>
-      </c>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
+      <c r="K4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>2</v>
+      </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>3</v>
-      </c>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
+      <c r="K5" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>3</v>
+      </c>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>3</v>
-      </c>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="K6" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>3</v>
+      </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="M8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="29"/>
+      <c r="P8" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="29"/>
+      <c r="S8" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="T8" s="29"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" s="15"/>
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="29"/>
+      <c r="M10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U10" s="15"/>
+      <c r="V10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="F11" s="31">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="6"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="29"/>
+      <c r="P14" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q14" s="22"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="G15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="I8" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="29"/>
-      <c r="L8" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="29"/>
-      <c r="O8" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="29"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="15"/>
-      <c r="R9">
+      <c r="H15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15" s="29"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="29"/>
-      <c r="I10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="1" t="s">
+      <c r="M17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I18" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="15"/>
-      <c r="R10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="J19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="4" t="s">
+      <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="29"/>
-      <c r="L14" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="22"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="29"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E18" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F24" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="K25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
       <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="N26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E27" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
       <c r="H27" s="30"/>
@@ -1849,244 +2589,254 @@
       <c r="P27" s="30"/>
       <c r="Q27" s="30"/>
       <c r="R27" s="30"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="26" t="s">
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F28" s="5"/>
+      <c r="G28" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
       <c r="H28" s="26"/>
-      <c r="J28" t="s">
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="N28" t="s">
         <v>5</v>
       </c>
-      <c r="M28" s="25" t="s">
+      <c r="Q28" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="N28" s="25"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="1">
+      <c r="R28" s="25"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F29" s="5"/>
+      <c r="G29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="L29" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M29" s="1">
-        <v>1</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="O29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>1</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M30" s="1">
-        <v>1</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J31" s="13" t="s">
+      <c r="O30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q30" s="1">
         <v>1</v>
       </c>
-      <c r="K31" s="10" t="s">
+      <c r="R30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N31" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="M31" s="1">
-        <v>2</v>
-      </c>
-      <c r="N31" s="1" t="s">
+      <c r="Q31" s="1">
+        <v>2</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
         <v>36</v>
       </c>
-      <c r="E32" t="s">
+      <c r="I32" t="s">
         <v>64</v>
       </c>
-      <c r="F32" t="s">
+      <c r="J32" t="s">
         <v>65</v>
       </c>
-      <c r="G32" t="s">
+      <c r="K32" t="s">
         <v>62</v>
       </c>
-      <c r="J32" s="9">
+      <c r="N32" s="9">
         <v>1</v>
       </c>
-      <c r="K32" s="9" t="s">
+      <c r="O32" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="L32">
+      <c r="P32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="9">
+    <row r="33" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H33" s="9">
         <v>1</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="F33" s="9">
-        <v>1</v>
-      </c>
-      <c r="G33" s="9">
-        <v>1</v>
-      </c>
-      <c r="H33" s="10">
-        <v>1</v>
       </c>
       <c r="J33" s="9">
         <v>1</v>
       </c>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="9">
+        <v>1</v>
+      </c>
+      <c r="L33" s="10">
+        <v>1</v>
+      </c>
+      <c r="N33" s="9">
+        <v>1</v>
+      </c>
+      <c r="O33" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="L33" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D34" s="12">
-        <v>2</v>
-      </c>
-      <c r="E34" s="12" t="s">
+      <c r="P33" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H34" s="12">
+        <v>2</v>
+      </c>
+      <c r="I34" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="12">
-        <v>2</v>
-      </c>
-      <c r="G34" s="12">
+      <c r="J34" s="12">
+        <v>2</v>
+      </c>
+      <c r="K34" s="12">
         <v>1</v>
       </c>
-      <c r="J34" s="11">
-        <v>2</v>
-      </c>
-      <c r="K34" s="11" t="s">
+      <c r="N34" s="11">
+        <v>2</v>
+      </c>
+      <c r="O34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L34">
+      <c r="P34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J35" s="11">
-        <v>2</v>
-      </c>
-      <c r="K35" s="11" t="s">
+    <row r="35" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="N35" s="11">
+        <v>2</v>
+      </c>
+      <c r="O35" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="P35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+    </row>
+    <row r="37" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>78</v>
+      </c>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+    </row>
+    <row r="38" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="1" t="s">
+    </row>
+    <row r="39" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="1">
-        <v>2</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+    <row r="41" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="E1:P1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A27:R27"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="O8:P8"/>
+  <mergeCells count="22">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B1:V1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="G28:L28"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E27:V27"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="S8:T8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>